<commit_message>
Fix sorting and generate viable xlsx and charts
</commit_message>
<xml_diff>
--- a/ReportData/PreparedDataPointChart/RandomFloat100_HeapSortTimes.csv.xlsx
+++ b/ReportData/PreparedDataPointChart/RandomFloat100_HeapSortTimes.csv.xlsx
@@ -184,10 +184,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.97829543</c:v>
+                  <c:v>0.84116882</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7768945</c:v>
+                  <c:v>1.8166705</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3.6254162</c:v>
@@ -641,7 +641,7 @@
         <v>100</v>
       </c>
       <c r="D2">
-        <v>0.97829543</v>
+        <v>0.84116882</v>
       </c>
       <c r="E2">
         <v>5000</v>
@@ -658,7 +658,7 @@
         <v>100</v>
       </c>
       <c r="D3">
-        <v>1.7768945</v>
+        <v>1.8166705</v>
       </c>
       <c r="E3">
         <v>10000</v>

</xml_diff>